<commit_message>
added first way of putting custom forms
</commit_message>
<xml_diff>
--- a/Nms_ADLIDs.xlsx
+++ b/Nms_ADLIDs.xlsx
@@ -5,13 +5,13 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="R8eb468b77b3a4789"/>
+    <sheet name="Sheet1" sheetId="1" r:id="R28ae299889ad42f1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="591">
   <si>
     <t>Client.ADLID</t>
   </si>
@@ -1730,9 +1730,6 @@
   </si>
   <si>
     <t>Mr Gary Goodwin</t>
-  </si>
-  <si>
-    <t>ADL6172022</t>
   </si>
   <si>
     <t>ADL6172925</t>
@@ -1897,7 +1894,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B297"/>
+  <dimension ref="A1:B296"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4208,79 +4205,71 @@
         <v>573</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>3</v>
+        <v>574</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="3" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="3" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="3" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="3" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="3" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="3" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="3" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="3" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="B297" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>